<commit_message>
Work with some new data from Jon's original experiment
</commit_message>
<xml_diff>
--- a/Examples_OnePond_TwoCatches_for_Jon.xlsx
+++ b/Examples_OnePond_TwoCatches_for_Jon.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="14625"/>
+    <workbookView xWindow="27740" yWindow="-460" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Library_Agg_data (88)" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2846,26 +2851,26 @@
   <dimension ref="A1:L185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D23"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -2903,7 +2908,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2941,7 +2946,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -2979,7 +2984,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -3017,7 +3022,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -3055,7 +3060,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -3093,7 +3098,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -3131,7 +3136,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -3169,7 +3174,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -3207,7 +3212,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -3245,7 +3250,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -3283,7 +3288,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -3321,7 +3326,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -3359,7 +3364,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -3397,7 +3402,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -3435,7 +3440,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -3473,7 +3478,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -3511,7 +3516,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -3549,7 +3554,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -3587,7 +3592,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -3625,7 +3630,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -3663,7 +3668,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -3701,7 +3706,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -3739,7 +3744,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -3777,7 +3782,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -3815,7 +3820,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -3853,7 +3858,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -3891,7 +3896,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -3929,7 +3934,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -3967,7 +3972,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -4005,7 +4010,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -4043,7 +4048,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -4081,7 +4086,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -4119,7 +4124,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -4157,7 +4162,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -4195,7 +4200,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -4233,7 +4238,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -4271,7 +4276,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12">
       <c r="A38" t="s">
         <v>18</v>
       </c>
@@ -4309,7 +4314,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -4347,7 +4352,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -4385,7 +4390,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -4423,7 +4428,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12">
       <c r="A42" t="s">
         <v>18</v>
       </c>
@@ -4461,7 +4466,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -4499,7 +4504,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12">
       <c r="A44" t="s">
         <v>18</v>
       </c>
@@ -4537,7 +4542,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12">
       <c r="A45" t="s">
         <v>18</v>
       </c>
@@ -4575,7 +4580,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12">
       <c r="A46" t="s">
         <v>18</v>
       </c>
@@ -4613,7 +4618,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -4651,7 +4656,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12">
       <c r="A48" t="s">
         <v>18</v>
       </c>
@@ -4689,7 +4694,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12">
       <c r="A49" t="s">
         <v>18</v>
       </c>
@@ -4727,7 +4732,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12">
       <c r="A50" t="s">
         <v>18</v>
       </c>
@@ -4765,7 +4770,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12">
       <c r="A51" t="s">
         <v>18</v>
       </c>
@@ -4803,7 +4808,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12">
       <c r="A52" t="s">
         <v>18</v>
       </c>
@@ -4841,7 +4846,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -4879,7 +4884,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12">
       <c r="A54" t="s">
         <v>18</v>
       </c>
@@ -4917,7 +4922,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12">
       <c r="A55" t="s">
         <v>18</v>
       </c>
@@ -4955,7 +4960,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -4993,7 +4998,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -5031,7 +5036,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -5069,7 +5074,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -5107,7 +5112,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12">
       <c r="A60" t="s">
         <v>18</v>
       </c>
@@ -5145,7 +5150,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12">
       <c r="A61" t="s">
         <v>18</v>
       </c>
@@ -5183,7 +5188,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12">
       <c r="A62" t="s">
         <v>18</v>
       </c>
@@ -5221,7 +5226,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12">
       <c r="A63" t="s">
         <v>18</v>
       </c>
@@ -5259,7 +5264,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12">
       <c r="A64" t="s">
         <v>18</v>
       </c>
@@ -5297,7 +5302,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12">
       <c r="A65" t="s">
         <v>18</v>
       </c>
@@ -5335,7 +5340,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12">
       <c r="A66" t="s">
         <v>18</v>
       </c>
@@ -5373,7 +5378,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12">
       <c r="A67" t="s">
         <v>18</v>
       </c>
@@ -5411,7 +5416,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12">
       <c r="A68" t="s">
         <v>18</v>
       </c>
@@ -5449,7 +5454,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12">
       <c r="A69" t="s">
         <v>18</v>
       </c>
@@ -5487,7 +5492,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12">
       <c r="A70" t="s">
         <v>18</v>
       </c>
@@ -5525,7 +5530,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12">
       <c r="A71" t="s">
         <v>18</v>
       </c>
@@ -5563,7 +5568,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12">
       <c r="A72" t="s">
         <v>18</v>
       </c>
@@ -5601,7 +5606,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12">
       <c r="A73" t="s">
         <v>18</v>
       </c>
@@ -5639,7 +5644,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12">
       <c r="A74" t="s">
         <v>18</v>
       </c>
@@ -5677,7 +5682,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12">
       <c r="A75" t="s">
         <v>18</v>
       </c>
@@ -5715,7 +5720,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12">
       <c r="A76" t="s">
         <v>18</v>
       </c>
@@ -5753,7 +5758,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12">
       <c r="A77" t="s">
         <v>18</v>
       </c>
@@ -5791,7 +5796,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12">
       <c r="A78" t="s">
         <v>18</v>
       </c>
@@ -5829,7 +5834,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12">
       <c r="A79" t="s">
         <v>18</v>
       </c>
@@ -5867,7 +5872,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12">
       <c r="A80" t="s">
         <v>18</v>
       </c>
@@ -5905,7 +5910,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12">
       <c r="A81" t="s">
         <v>18</v>
       </c>
@@ -5943,7 +5948,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12">
       <c r="A82" t="s">
         <v>18</v>
       </c>
@@ -5981,7 +5986,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12">
       <c r="A83" t="s">
         <v>18</v>
       </c>
@@ -6019,7 +6024,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12">
       <c r="A84" t="s">
         <v>18</v>
       </c>
@@ -6057,7 +6062,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12">
       <c r="A85" t="s">
         <v>18</v>
       </c>
@@ -6095,7 +6100,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12">
       <c r="A86" t="s">
         <v>18</v>
       </c>
@@ -6133,7 +6138,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12">
       <c r="A87" t="s">
         <v>18</v>
       </c>
@@ -6171,7 +6176,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12">
       <c r="A88" t="s">
         <v>18</v>
       </c>
@@ -6209,7 +6214,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12">
       <c r="A89" t="s">
         <v>18</v>
       </c>
@@ -6247,7 +6252,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12">
       <c r="A90" t="s">
         <v>18</v>
       </c>
@@ -6285,7 +6290,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12">
       <c r="A91" t="s">
         <v>18</v>
       </c>
@@ -6323,7 +6328,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12">
       <c r="A92" t="s">
         <v>18</v>
       </c>
@@ -6361,7 +6366,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12">
       <c r="A93" t="s">
         <v>18</v>
       </c>
@@ -6399,7 +6404,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12">
       <c r="A94" t="s">
         <v>18</v>
       </c>
@@ -6437,7 +6442,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12">
       <c r="A95" t="s">
         <v>18</v>
       </c>
@@ -6475,7 +6480,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12">
       <c r="A96" t="s">
         <v>18</v>
       </c>
@@ -6513,7 +6518,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12">
       <c r="A97" t="s">
         <v>18</v>
       </c>
@@ -6551,7 +6556,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12">
       <c r="A98" t="s">
         <v>18</v>
       </c>
@@ -6589,7 +6594,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12">
       <c r="A99" t="s">
         <v>18</v>
       </c>
@@ -6627,7 +6632,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12">
       <c r="A100" t="s">
         <v>18</v>
       </c>
@@ -6665,7 +6670,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12">
       <c r="A101" t="s">
         <v>18</v>
       </c>
@@ -6703,7 +6708,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12">
       <c r="A102" t="s">
         <v>18</v>
       </c>
@@ -6741,7 +6746,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12">
       <c r="A103" t="s">
         <v>18</v>
       </c>
@@ -6779,7 +6784,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12">
       <c r="A104" t="s">
         <v>18</v>
       </c>
@@ -6817,7 +6822,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12">
       <c r="A105" t="s">
         <v>18</v>
       </c>
@@ -6855,7 +6860,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12">
       <c r="A106" t="s">
         <v>18</v>
       </c>
@@ -6893,7 +6898,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12">
       <c r="A107" t="s">
         <v>18</v>
       </c>
@@ -6931,7 +6936,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12">
       <c r="A108" t="s">
         <v>18</v>
       </c>
@@ -6969,7 +6974,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12">
       <c r="A109" t="s">
         <v>18</v>
       </c>
@@ -7007,7 +7012,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12">
       <c r="A110" t="s">
         <v>18</v>
       </c>
@@ -7045,7 +7050,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12">
       <c r="A111" t="s">
         <v>18</v>
       </c>
@@ -7083,7 +7088,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12">
       <c r="A112" t="s">
         <v>18</v>
       </c>
@@ -7121,7 +7126,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12">
       <c r="A113" t="s">
         <v>18</v>
       </c>
@@ -7159,7 +7164,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12">
       <c r="A114" t="s">
         <v>18</v>
       </c>
@@ -7197,7 +7202,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12">
       <c r="A115" t="s">
         <v>18</v>
       </c>
@@ -7235,7 +7240,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12">
       <c r="A116" t="s">
         <v>18</v>
       </c>
@@ -7273,7 +7278,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12">
       <c r="A117" t="s">
         <v>18</v>
       </c>
@@ -7311,7 +7316,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12">
       <c r="A118" t="s">
         <v>18</v>
       </c>
@@ -7349,7 +7354,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12">
       <c r="A119" t="s">
         <v>18</v>
       </c>
@@ -7387,7 +7392,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12">
       <c r="A120" t="s">
         <v>18</v>
       </c>
@@ -7425,7 +7430,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12">
       <c r="A121" t="s">
         <v>18</v>
       </c>
@@ -7463,7 +7468,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12">
       <c r="A122" t="s">
         <v>18</v>
       </c>
@@ -7501,7 +7506,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12">
       <c r="A123" t="s">
         <v>18</v>
       </c>
@@ -7539,7 +7544,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12">
       <c r="A124" t="s">
         <v>18</v>
       </c>
@@ -7577,7 +7582,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12">
       <c r="A125" t="s">
         <v>18</v>
       </c>
@@ -7615,7 +7620,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12">
       <c r="A126" t="s">
         <v>18</v>
       </c>
@@ -7653,7 +7658,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12">
       <c r="A127" t="s">
         <v>18</v>
       </c>
@@ -7691,7 +7696,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12">
       <c r="A128" t="s">
         <v>18</v>
       </c>
@@ -7729,7 +7734,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12">
       <c r="A129" t="s">
         <v>18</v>
       </c>
@@ -7767,7 +7772,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12">
       <c r="A130" t="s">
         <v>18</v>
       </c>
@@ -7805,7 +7810,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12">
       <c r="A131" t="s">
         <v>18</v>
       </c>
@@ -7843,7 +7848,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12">
       <c r="A132" t="s">
         <v>18</v>
       </c>
@@ -7881,7 +7886,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12">
       <c r="A133" t="s">
         <v>18</v>
       </c>
@@ -7919,7 +7924,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12">
       <c r="A134" t="s">
         <v>18</v>
       </c>
@@ -7957,7 +7962,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12">
       <c r="A135" t="s">
         <v>18</v>
       </c>
@@ -7995,7 +8000,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12">
       <c r="A136" t="s">
         <v>18</v>
       </c>
@@ -8033,7 +8038,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12">
       <c r="A137" t="s">
         <v>18</v>
       </c>
@@ -8071,7 +8076,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12">
       <c r="A138" t="s">
         <v>18</v>
       </c>
@@ -8109,7 +8114,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12">
       <c r="A139" t="s">
         <v>18</v>
       </c>
@@ -8147,7 +8152,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12">
       <c r="A140" t="s">
         <v>18</v>
       </c>
@@ -8185,7 +8190,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12">
       <c r="A141" t="s">
         <v>18</v>
       </c>
@@ -8223,7 +8228,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12">
       <c r="A142" t="s">
         <v>18</v>
       </c>
@@ -8261,7 +8266,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12">
       <c r="A143" t="s">
         <v>18</v>
       </c>
@@ -8299,7 +8304,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12">
       <c r="A144" t="s">
         <v>18</v>
       </c>
@@ -8337,7 +8342,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12">
       <c r="A145" t="s">
         <v>18</v>
       </c>
@@ -8375,7 +8380,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12">
       <c r="A146" t="s">
         <v>18</v>
       </c>
@@ -8413,7 +8418,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12">
       <c r="A147" t="s">
         <v>18</v>
       </c>
@@ -8451,7 +8456,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12">
       <c r="A148" t="s">
         <v>18</v>
       </c>
@@ -8489,7 +8494,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12">
       <c r="A149" t="s">
         <v>18</v>
       </c>
@@ -8527,7 +8532,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12">
       <c r="A150" t="s">
         <v>18</v>
       </c>
@@ -8565,7 +8570,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12">
       <c r="A151" t="s">
         <v>18</v>
       </c>
@@ -8603,7 +8608,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12">
       <c r="A152" t="s">
         <v>18</v>
       </c>
@@ -8641,7 +8646,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12">
       <c r="A153" t="s">
         <v>18</v>
       </c>
@@ -8679,7 +8684,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12">
       <c r="A154" t="s">
         <v>18</v>
       </c>
@@ -8717,7 +8722,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12">
       <c r="A155" t="s">
         <v>18</v>
       </c>
@@ -8755,7 +8760,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12">
       <c r="A156" t="s">
         <v>18</v>
       </c>
@@ -8793,7 +8798,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12">
       <c r="A157" t="s">
         <v>18</v>
       </c>
@@ -8831,7 +8836,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12">
       <c r="A158" t="s">
         <v>18</v>
       </c>
@@ -8869,7 +8874,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12">
       <c r="A159" t="s">
         <v>18</v>
       </c>
@@ -8907,7 +8912,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12">
       <c r="A160" t="s">
         <v>18</v>
       </c>
@@ -8945,7 +8950,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12">
       <c r="A161" t="s">
         <v>18</v>
       </c>
@@ -8983,7 +8988,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12">
       <c r="A162" t="s">
         <v>18</v>
       </c>
@@ -9021,7 +9026,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12">
       <c r="A163" t="s">
         <v>18</v>
       </c>
@@ -9059,7 +9064,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12">
       <c r="A164" t="s">
         <v>18</v>
       </c>
@@ -9097,7 +9102,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12">
       <c r="A165" t="s">
         <v>18</v>
       </c>
@@ -9135,7 +9140,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12">
       <c r="A166" t="s">
         <v>18</v>
       </c>
@@ -9173,7 +9178,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12">
       <c r="A167" t="s">
         <v>18</v>
       </c>
@@ -9211,7 +9216,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12">
       <c r="A168" t="s">
         <v>18</v>
       </c>
@@ -9249,7 +9254,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12">
       <c r="A169" t="s">
         <v>18</v>
       </c>
@@ -9287,7 +9292,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12">
       <c r="A170" t="s">
         <v>18</v>
       </c>
@@ -9325,7 +9330,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12">
       <c r="A171" t="s">
         <v>18</v>
       </c>
@@ -9363,7 +9368,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12">
       <c r="A172" t="s">
         <v>18</v>
       </c>
@@ -9401,7 +9406,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12">
       <c r="A173" t="s">
         <v>18</v>
       </c>
@@ -9439,7 +9444,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12">
       <c r="A174" t="s">
         <v>18</v>
       </c>
@@ -9477,7 +9482,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12">
       <c r="A175" t="s">
         <v>18</v>
       </c>
@@ -9515,7 +9520,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12">
       <c r="A176" t="s">
         <v>18</v>
       </c>
@@ -9553,7 +9558,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12">
       <c r="A177" t="s">
         <v>18</v>
       </c>
@@ -9591,7 +9596,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12">
       <c r="A178" t="s">
         <v>18</v>
       </c>
@@ -9629,7 +9634,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12">
       <c r="A179" t="s">
         <v>18</v>
       </c>
@@ -9667,7 +9672,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12">
       <c r="A180" t="s">
         <v>18</v>
       </c>
@@ -9705,7 +9710,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12">
       <c r="A181" t="s">
         <v>18</v>
       </c>
@@ -9743,7 +9748,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12">
       <c r="A182" t="s">
         <v>18</v>
       </c>
@@ -9781,7 +9786,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12">
       <c r="A183" t="s">
         <v>18</v>
       </c>
@@ -9819,7 +9824,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12">
       <c r="A184" t="s">
         <v>18</v>
       </c>
@@ -9857,7 +9862,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12">
       <c r="A185" t="s">
         <v>18</v>
       </c>
@@ -9901,5 +9906,10 @@
     <sortCondition ref="D2:D185"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>